<commit_message>
Updated Code ~Foxit handled
</commit_message>
<xml_diff>
--- a/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
+++ b/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
@@ -1,44 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\source\repos\ExcelHierarchyConversion_InterOp\ExcelHierarchyConversion_InterOp\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\006 - Hierarchy Converter V3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D733583-5F1A-42F1-86DD-0467B9990506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Function!$A$1:$AV$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Function!$A$1:$AW$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Code</t>
   </si>
@@ -155,12 +145,15 @@
   </si>
   <si>
     <t>Maximo Equipment Description</t>
+  </si>
+  <si>
+    <t>Round Title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
@@ -273,7 +266,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -584,63 +577,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="45.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="67.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="70.77734375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="70.77734375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.5703125" style="2" customWidth="1"/>
-    <col min="41" max="41" width="14.140625" style="2" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="2"/>
+    <col min="28" max="28" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="14.88671875" style="2" customWidth="1"/>
+    <col min="33" max="33" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.33203125" style="2" customWidth="1"/>
+    <col min="38" max="38" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.5546875" style="2" customWidth="1"/>
+    <col min="42" max="42" width="14.109375" style="2" customWidth="1"/>
+    <col min="43" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -735,30 +728,32 @@
         <v>28</v>
       </c>
       <c r="AF1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="9"/>
       <c r="AO1" s="9"/>
       <c r="AP1" s="9"/>
       <c r="AQ1" s="9"/>
@@ -767,30 +762,31 @@
       <c r="AT1" s="9"/>
       <c r="AU1" s="9"/>
       <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="K2" s="3"/>
-      <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Generic Model details not required, Details Required, Not Required Components Will Never Be installed, Details Provided are Correct, Remove"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL1:AL1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM1:AM1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM1:AM1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN1:AN1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Yes,Hold,Discard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ1:AJ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK1:AK1048576" xr:uid="{DF1DEDD5-7AC9-46D9-886F-7F8187384363}">
       <formula1>"Company's Requirement, Fleet Maintenance System, Maker's Manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1:AF1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG1:AG1048576" xr:uid="{E5E290CC-3601-4AB3-8788-A604848A3F43}">
       <formula1>"Scheduled, Occasional, Fixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1:AD1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1:AD1048576" xr:uid="{E1034F9F-3A07-4591-BCEC-DF1D3B459508}">
       <formula1>"Engine, Deck, Electrical"</formula1>
     </dataValidation>
   </dataValidations>
@@ -810,6 +806,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c85056a-e6fd-4f75-9e79-2fe4acc5d342">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="bf893fa4-83d1-42b8-a141-583783f5dadd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100069957EBFE0C234A836383065DAFD646" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bdcaeb6b2a15e266e67c4fa9d46e185">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6c85056a-e6fd-4f75-9e79-2fe4acc5d342" xmlns:ns3="bf893fa4-83d1-42b8-a141-583783f5dadd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="974284ad07c58caadee2618c32b7db20" ns2:_="" ns3:_="">
     <xsd:import namespace="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
@@ -1038,17 +1045,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c85056a-e6fd-4f75-9e79-2fe4acc5d342">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="bf893fa4-83d1-42b8-a141-583783f5dadd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
   <ds:schemaRefs>
@@ -1058,6 +1054,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14403433-4C24-422F-B99C-E1EC12E98015}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
+    <ds:schemaRef ds:uri="bf893fa4-83d1-42b8-a141-583783f5dadd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22853306-49CC-4C73-87A1-B39EF4C8BD4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1074,15 +1081,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14403433-4C24-422F-B99C-E1EC12E98015}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
-    <ds:schemaRef ds:uri="bf893fa4-83d1-42b8-a141-583783f5dadd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Code Left split
</commit_message>
<xml_diff>
--- a/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
+++ b/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
@@ -1,34 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\006 - Hierarchy Converter V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\source\repos\ExcelHierarchyConversion_InterOp\ExcelHierarchyConversion_InterOp\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D733583-5F1A-42F1-86DD-0467B9990506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Function!$A$1:$AW$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Function!$A$1:$AV$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Code</t>
   </si>
@@ -145,15 +155,12 @@
   </si>
   <si>
     <t>Maximo Equipment Description</t>
-  </si>
-  <si>
-    <t>Round Title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
@@ -234,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -263,10 +270,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -577,64 +587,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S16" sqref="S16"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="32.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="67.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="70.77734375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="70.77734375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="45.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="14.88671875" style="2" customWidth="1"/>
-    <col min="33" max="33" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.33203125" style="2" customWidth="1"/>
-    <col min="38" max="38" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.5546875" style="2" customWidth="1"/>
-    <col min="42" max="42" width="14.109375" style="2" customWidth="1"/>
-    <col min="43" max="16384" width="9.109375" style="2"/>
+    <col min="28" max="28" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.5703125" style="2" customWidth="1"/>
+    <col min="41" max="41" width="14.140625" style="2" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:48" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -728,32 +738,30 @@
         <v>28</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG1" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="AG1" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="AH1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AJ1" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="AK1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="AL1" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="AM1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN1" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="AN1" s="9"/>
       <c r="AO1" s="9"/>
       <c r="AP1" s="9"/>
       <c r="AQ1" s="9"/>
@@ -762,31 +770,30 @@
       <c r="AT1" s="9"/>
       <c r="AU1" s="9"/>
       <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="K2" s="3"/>
+      <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576">
       <formula1>"Generic Model details not required, Details Required, Not Required Components Will Never Be installed, Details Provided are Correct, Remove"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM1:AM1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL1:AL1048576">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN1:AN1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM1:AM1048576">
       <formula1>"Yes,Hold,Discard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK1:AK1048576" xr:uid="{DF1DEDD5-7AC9-46D9-886F-7F8187384363}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ1:AJ1048576">
       <formula1>"Company's Requirement, Fleet Maintenance System, Maker's Manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG1:AG1048576" xr:uid="{E5E290CC-3601-4AB3-8788-A604848A3F43}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1:AF1048576">
       <formula1>"Scheduled, Occasional, Fixed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1:AD1048576" xr:uid="{E1034F9F-3A07-4591-BCEC-DF1D3B459508}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1:AD1048576">
       <formula1>"Engine, Deck, Electrical"</formula1>
     </dataValidation>
   </dataValidations>
@@ -797,15 +804,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c85056a-e6fd-4f75-9e79-2fe4acc5d342">
@@ -816,7 +814,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100069957EBFE0C234A836383065DAFD646" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bdcaeb6b2a15e266e67c4fa9d46e185">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6c85056a-e6fd-4f75-9e79-2fe4acc5d342" xmlns:ns3="bf893fa4-83d1-42b8-a141-583783f5dadd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="974284ad07c58caadee2618c32b7db20" ns2:_="" ns3:_="">
     <xsd:import namespace="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
@@ -1045,15 +1043,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14403433-4C24-422F-B99C-E1EC12E98015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1064,7 +1063,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22853306-49CC-4C73-87A1-B39EF4C8BD4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1081,4 +1080,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Code fixed Bugs Related to output Sheet Com left
</commit_message>
<xml_diff>
--- a/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
+++ b/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Function!$A$1:$AV$2</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Code</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Maximo Equipment Description</t>
+  </si>
+  <si>
+    <t>Data Id</t>
   </si>
 </sst>
 </file>
@@ -591,10 +594,10 @@
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection pane="bottomRight" activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -638,7 +641,7 @@
     <col min="37" max="37" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.5703125" style="2" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="14.140625" style="2" customWidth="1"/>
     <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -761,7 +764,9 @@
       <c r="AM1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="9"/>
+      <c r="AN1" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="AO1" s="9"/>
       <c r="AP1" s="9"/>
       <c r="AQ1" s="9"/>
@@ -804,14 +809,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c85056a-e6fd-4f75-9e79-2fe4acc5d342">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="bf893fa4-83d1-42b8-a141-583783f5dadd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1044,21 +1047,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6c85056a-e6fd-4f75-9e79-2fe4acc5d342">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="bf893fa4-83d1-42b8-a141-583783f5dadd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14403433-4C24-422F-B99C-E1EC12E98015}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
-    <ds:schemaRef ds:uri="bf893fa4-83d1-42b8-a141-583783f5dadd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1083,9 +1085,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14403433-4C24-422F-B99C-E1EC12E98015}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
+    <ds:schemaRef ds:uri="bf893fa4-83d1-42b8-a141-583783f5dadd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final Code working in my machine
</commit_message>
<xml_diff>
--- a/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
+++ b/ExcelHierarchyConversion_InterOp/bin/Debug/Output Template.xlsx
@@ -597,7 +597,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL15" sqref="AL15"/>
+      <selection pane="bottomRight" activeCell="AG1" sqref="AG1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -634,7 +634,7 @@
     <col min="30" max="30" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -743,7 +743,7 @@
       <c r="AF1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="10" t="s">
         <v>30</v>
       </c>
       <c r="AH1" s="5" t="s">
@@ -778,7 +778,6 @@
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="K2" s="3"/>
-      <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
     </row>
   </sheetData>
@@ -809,15 +808,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100069957EBFE0C234A836383065DAFD646" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bdcaeb6b2a15e266e67c4fa9d46e185">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6c85056a-e6fd-4f75-9e79-2fe4acc5d342" xmlns:ns3="bf893fa4-83d1-42b8-a141-583783f5dadd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="974284ad07c58caadee2618c32b7db20" ns2:_="" ns3:_="">
     <xsd:import namespace="6c85056a-e6fd-4f75-9e79-2fe4acc5d342"/>
@@ -1046,6 +1036,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1058,14 +1057,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22853306-49CC-4C73-87A1-B39EF4C8BD4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1084,6 +1075,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD2FACE-E618-4C1F-8671-B67E661DFE47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14403433-4C24-422F-B99C-E1EC12E98015}">
   <ds:schemaRefs>

</xml_diff>